<commit_message>
[API] (Landlod - Add multiple room)
Update file Excel & condition
</commit_message>
<xml_diff>
--- a/HouseFinder_API/HouseFinder_API/house-template.xlsx
+++ b/HouseFinder_API/HouseFinder_API/house-template.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\fu-house-finder\HouseFinder_API\HouseFinder_API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Semester9\SEP490\fu-house-finder\HouseFinder_API\HouseFinder_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397938BA-54D6-4ADC-AF4F-8F286969A87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9885F2E1-C928-449D-8605-0F1F367D478D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54A03348-2A5B-4965-B635-BEB8F37FAFD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{54A03348-2A5B-4965-B635-BEB8F37FAFD6}"/>
   </bookViews>
   <sheets>
     <sheet name="DANH SÁCH PHÒNG" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Tòa nhà</t>
   </si>
@@ -47,12 +36,6 @@
     <t>Tên phòng</t>
   </si>
   <si>
-    <t>Giá phòng</t>
-  </si>
-  <si>
-    <t>Diện tích phòng</t>
-  </si>
-  <si>
     <t>Số người tối đa</t>
   </si>
   <si>
@@ -80,20 +63,29 @@
     <t>Chung chủ</t>
   </si>
   <si>
-    <t>Thông tin phòng</t>
-  </si>
-  <si>
     <t>Số người hiện tại</t>
   </si>
   <si>
     <t>Loại phòng</t>
+  </si>
+  <si>
+    <t>DANH SÁCH PHÒNG TRỌ</t>
+  </si>
+  <si>
+    <t>Diện tích phòng (m2)</t>
+  </si>
+  <si>
+    <t>Thông tin thêm</t>
+  </si>
+  <si>
+    <t>Giá phòng (VNĐ)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,16 +93,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,16 +132,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -444,116 +480,455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA55082-9BB4-4B5C-9788-89AC9E9249E0}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="7.21875" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
+  <mergeCells count="11">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:P1048576" xr:uid="{B83EBEFB-07D4-4AAA-B8AF-1A334119AA12}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:P1048576" xr:uid="{B83EBEFB-07D4-4AAA-B8AF-1A334119AA12}">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:B1048576 G3:G1048576 E3:F1048576" xr:uid="{22B3F831-D0A5-4867-840B-86D7BA231C5D}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:B1048576 G4:G1048576 E4:F1048576" xr:uid="{22B3F831-D0A5-4867-840B-86D7BA231C5D}">
       <formula1>0</formula1>
       <formula2>9999</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{154AAB61-E7D1-4DEC-8B62-A1EDE2C97338}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H1048576" xr:uid="{154AAB61-E7D1-4DEC-8B62-A1EDE2C97338}">
       <formula1>"Khép kín, Không khép kín, Chung cư mini"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576" xr:uid="{9E0E8182-D848-46FB-9963-0B5C5257C5A2}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D1048576" xr:uid="{9E0E8182-D848-46FB-9963-0B5C5257C5A2}">
       <formula1>0</formula1>
       <formula2>9999999999</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>